<commit_message>
Implemented extension to non-diag chi
</commit_message>
<xml_diff>
--- a/data/hyperfines_and_shifts_298.xlsx
+++ b/data/hyperfines_and_shifts_298.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danburrows/Documents/Codes/simpNMR/simpnmr/simpnmr/sandbox_experiments/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danburrows/Documents/Codes/simpNMR/simpnmr/simpnmr/sandbox_experiments/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF20E83D-D37A-5242-B7D5-344EB1E784A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB96C4F3-9946-D149-A9FB-7FC75EF4112B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29120" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31440" yWindow="7040" windowWidth="29120" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - hyperfines_and_shifts" sheetId="1" r:id="rId1"/>
@@ -1634,7 +1634,7 @@
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>